<commit_message>
fixed ap mode and added time sync from phone/pc
</commit_message>
<xml_diff>
--- a/docs/Wortuhr_worte.xlsx
+++ b/docs/Wortuhr_worte.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\NAS\Michael\Geschenke\Weihnachten\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\NAS\Michael\Hobby\Microkontroller\Wortuhr\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3060ACC-9368-4E4B-A9B9-60FBF0E9D3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C023A061-306B-4256-BCFB-95095E0EBEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7B3A79A3-EA99-4882-92CE-2951A4ABBE17}"/>
   </bookViews>
@@ -199,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,7 +208,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -656,9 +662,6 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -684,15 +687,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -709,24 +703,51 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -736,61 +757,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1124,14 +1100,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="84.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" s="20" t="s">
+      <c r="Z1" s="16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1161,87 +1137,87 @@
       <c r="L2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="49" t="s">
+      <c r="O2" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="50" t="s">
+      <c r="P2" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="51" t="s">
+      <c r="Q2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="52" t="s">
+      <c r="R2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="52" t="s">
+      <c r="S2" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="53" t="s">
+      <c r="T2" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="54" t="s">
+      <c r="U2" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="51" t="s">
+      <c r="V2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="52" t="s">
+      <c r="W2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="52" t="s">
+      <c r="X2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="55" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="24"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="23"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="7"/>
-      <c r="O3" s="55">
-        <v>0</v>
-      </c>
-      <c r="P3" s="56">
+      <c r="O3" s="37">
+        <v>0</v>
+      </c>
+      <c r="P3" s="38">
         <v>1</v>
       </c>
-      <c r="Q3" s="57">
+      <c r="Q3" s="39">
         <v>2</v>
       </c>
-      <c r="R3" s="58">
+      <c r="R3" s="40">
         <v>3</v>
       </c>
-      <c r="S3" s="58">
+      <c r="S3" s="40">
         <v>4</v>
       </c>
-      <c r="T3" s="59">
+      <c r="T3" s="41">
         <v>5</v>
       </c>
-      <c r="U3" s="60">
+      <c r="U3" s="42">
         <v>6</v>
       </c>
-      <c r="V3" s="57">
+      <c r="V3" s="39">
         <v>7</v>
       </c>
-      <c r="W3" s="58">
+      <c r="W3" s="40">
         <v>8</v>
       </c>
-      <c r="X3" s="58">
+      <c r="X3" s="40">
         <v>9</v>
       </c>
-      <c r="Y3" s="59">
+      <c r="Y3" s="41">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1275,41 +1251,41 @@
       <c r="L4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="51" t="s">
+      <c r="O4" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="52" t="s">
+      <c r="P4" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="53" t="s">
+      <c r="R4" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="51" t="s">
+      <c r="S4" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="52" t="s">
+      <c r="T4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="52" t="s">
+      <c r="U4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="52" t="s">
+      <c r="V4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="W4" s="52" t="s">
+      <c r="W4" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="X4" s="52" t="s">
+      <c r="X4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="Y4" s="53" t="s">
+      <c r="Y4" s="55" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1321,41 +1297,41 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="4"/>
-      <c r="O5" s="61">
+      <c r="O5" s="43">
         <v>21</v>
       </c>
-      <c r="P5" s="62">
+      <c r="P5" s="44">
         <v>20</v>
       </c>
-      <c r="Q5" s="62">
+      <c r="Q5" s="44">
         <v>19</v>
       </c>
-      <c r="R5" s="63">
+      <c r="R5" s="45">
         <v>18</v>
       </c>
-      <c r="S5" s="61">
+      <c r="S5" s="43">
         <v>17</v>
       </c>
-      <c r="T5" s="62">
+      <c r="T5" s="44">
         <v>16</v>
       </c>
-      <c r="U5" s="62">
+      <c r="U5" s="44">
         <v>15</v>
       </c>
-      <c r="V5" s="62">
+      <c r="V5" s="44">
         <v>14</v>
       </c>
-      <c r="W5" s="62">
+      <c r="W5" s="44">
         <v>13</v>
       </c>
-      <c r="X5" s="62">
+      <c r="X5" s="44">
         <v>12</v>
       </c>
-      <c r="Y5" s="63">
+      <c r="Y5" s="45">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1389,87 +1365,87 @@
       <c r="L6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="40" t="s">
+      <c r="O6" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="42" t="s">
+      <c r="P6" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="44" t="s">
+      <c r="Q6" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" s="46" t="s">
+      <c r="R6" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="T6" s="46" t="s">
+      <c r="T6" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="46" t="s">
+      <c r="U6" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="V6" s="49" t="s">
+      <c r="V6" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="W6" s="39" t="s">
+      <c r="W6" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="X6" s="39" t="s">
+      <c r="X6" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="Y6" s="39" t="s">
+      <c r="Y6" s="55" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="21"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="17"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="4"/>
-      <c r="O7" s="41">
+      <c r="O7" s="48">
         <v>22</v>
       </c>
-      <c r="P7" s="43">
+      <c r="P7" s="49">
         <v>23</v>
       </c>
-      <c r="Q7" s="45">
+      <c r="Q7" s="50">
         <v>24</v>
       </c>
-      <c r="R7" s="64">
+      <c r="R7" s="46">
         <v>25</v>
       </c>
-      <c r="S7" s="47">
+      <c r="S7" s="52">
         <v>26</v>
       </c>
-      <c r="T7" s="47">
+      <c r="T7" s="52">
         <v>27</v>
       </c>
-      <c r="U7" s="47">
+      <c r="U7" s="52">
         <v>28</v>
       </c>
-      <c r="V7" s="65">
+      <c r="V7" s="43">
         <v>29</v>
       </c>
-      <c r="W7" s="48">
+      <c r="W7" s="49">
         <v>30</v>
       </c>
-      <c r="X7" s="48">
+      <c r="X7" s="49">
         <v>31</v>
       </c>
-      <c r="Y7" s="48">
+      <c r="Y7" s="50">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
@@ -1495,87 +1471,87 @@
       <c r="L8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="40" t="s">
+      <c r="O8" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="52" t="s">
+      <c r="P8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="R8" s="52" t="s">
+      <c r="Q8" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="S8" s="42" t="s">
+      <c r="S8" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="T8" s="52" t="s">
+      <c r="T8" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="U8" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="V8" s="52" t="s">
+      <c r="U8" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="V8" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="W8" s="42" t="s">
+      <c r="W8" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="X8" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="44" t="s">
+      <c r="X8" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="55" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="3"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="4"/>
-      <c r="O9" s="41">
+      <c r="O9" s="48">
         <v>43</v>
       </c>
-      <c r="P9" s="62">
+      <c r="P9" s="44">
         <v>42</v>
       </c>
-      <c r="Q9" s="43">
+      <c r="Q9" s="49">
         <v>41</v>
       </c>
-      <c r="R9" s="62">
+      <c r="R9" s="44">
         <v>40</v>
       </c>
-      <c r="S9" s="43">
+      <c r="S9" s="49">
         <v>39</v>
       </c>
-      <c r="T9" s="62">
+      <c r="T9" s="44">
         <v>38</v>
       </c>
-      <c r="U9" s="43">
+      <c r="U9" s="49">
         <v>37</v>
       </c>
-      <c r="V9" s="62">
+      <c r="V9" s="44">
         <v>36</v>
       </c>
-      <c r="W9" s="43">
+      <c r="W9" s="49">
         <v>35</v>
       </c>
-      <c r="X9" s="62">
+      <c r="X9" s="44">
         <v>34</v>
       </c>
-      <c r="Y9" s="45">
+      <c r="Y9" s="50">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1603,87 +1579,87 @@
       <c r="L10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O10" s="40" t="s">
+      <c r="O10" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="42" t="s">
+      <c r="P10" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="Q10" s="42" t="s">
+      <c r="Q10" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="R10" s="53" t="s">
+      <c r="R10" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="S10" s="46" t="s">
+      <c r="S10" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="T10" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="U10" s="42" t="s">
+      <c r="T10" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="U10" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="V10" s="49" t="s">
+      <c r="V10" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="W10" s="42" t="s">
+      <c r="W10" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="X10" s="42" t="s">
+      <c r="X10" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="Y10" s="44" t="s">
+      <c r="Y10" s="55" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="4"/>
       <c r="F11" s="8"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="26"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="3"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="4"/>
-      <c r="O11" s="41">
+      <c r="O11" s="48">
         <v>44</v>
       </c>
-      <c r="P11" s="43">
+      <c r="P11" s="49">
         <v>45</v>
       </c>
-      <c r="Q11" s="43">
+      <c r="Q11" s="49">
         <v>46</v>
       </c>
-      <c r="R11" s="63">
+      <c r="R11" s="45">
         <v>47</v>
       </c>
-      <c r="S11" s="47">
+      <c r="S11" s="52">
         <v>48</v>
       </c>
-      <c r="T11" s="41">
+      <c r="T11" s="48">
         <v>49</v>
       </c>
-      <c r="U11" s="43">
+      <c r="U11" s="49">
         <v>50</v>
       </c>
-      <c r="V11" s="66">
+      <c r="V11" s="47">
         <v>51</v>
       </c>
-      <c r="W11" s="43">
+      <c r="W11" s="49">
         <v>52</v>
       </c>
-      <c r="X11" s="43">
+      <c r="X11" s="49">
         <v>53</v>
       </c>
-      <c r="Y11" s="45">
+      <c r="Y11" s="50">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1715,87 +1691,87 @@
       <c r="L12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O12" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="P12" s="31" t="s">
+      <c r="O12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="Q12" s="42" t="s">
+      <c r="Q12" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="R12" s="31" t="s">
+      <c r="R12" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="S12" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="T12" s="36" t="s">
+      <c r="S12" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="U12" s="40" t="s">
+      <c r="U12" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="V12" s="31" t="s">
+      <c r="V12" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="W12" s="42" t="s">
+      <c r="W12" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="X12" s="31" t="s">
+      <c r="X12" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="Y12" s="44" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y12" s="55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="22"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="21"/>
       <c r="I13" s="3"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="4"/>
-      <c r="O13" s="41">
+      <c r="O13" s="48">
         <v>65</v>
       </c>
-      <c r="P13" s="34">
+      <c r="P13" s="30">
         <v>64</v>
       </c>
-      <c r="Q13" s="43">
+      <c r="Q13" s="49">
         <v>63</v>
       </c>
-      <c r="R13" s="34">
+      <c r="R13" s="30">
         <v>62</v>
       </c>
-      <c r="S13" s="45">
+      <c r="S13" s="50">
         <v>61</v>
       </c>
-      <c r="T13" s="29">
+      <c r="T13" s="28">
         <v>60</v>
       </c>
-      <c r="U13" s="41">
+      <c r="U13" s="48">
         <v>59</v>
       </c>
-      <c r="V13" s="34">
+      <c r="V13" s="30">
         <v>58</v>
       </c>
-      <c r="W13" s="43">
+      <c r="W13" s="49">
         <v>57</v>
       </c>
-      <c r="X13" s="34">
+      <c r="X13" s="30">
         <v>56</v>
       </c>
-      <c r="Y13" s="45">
+      <c r="Y13" s="50">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1827,87 +1803,87 @@
       <c r="L14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O14" s="40" t="s">
+      <c r="O14" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="P14" s="42" t="s">
+      <c r="P14" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="Q14" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="R14" s="31" t="s">
+      <c r="Q14" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="S14" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="T14" s="46" t="s">
+      <c r="S14" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="T14" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="U14" s="40" t="s">
+      <c r="U14" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="V14" s="31" t="s">
+      <c r="V14" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="W14" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="X14" s="42" t="s">
+      <c r="W14" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="X14" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="Y14" s="44" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y14" s="55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="15"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
       <c r="I15" s="6"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="7"/>
-      <c r="O15" s="41">
+      <c r="O15" s="48">
         <v>66</v>
       </c>
-      <c r="P15" s="43">
+      <c r="P15" s="49">
         <v>67</v>
       </c>
-      <c r="Q15" s="43">
+      <c r="Q15" s="49">
         <v>68</v>
       </c>
-      <c r="R15" s="34">
+      <c r="R15" s="30">
         <v>69</v>
       </c>
-      <c r="S15" s="45">
+      <c r="S15" s="50">
         <v>70</v>
       </c>
-      <c r="T15" s="47">
+      <c r="T15" s="52">
         <v>71</v>
       </c>
-      <c r="U15" s="41">
+      <c r="U15" s="48">
         <v>72</v>
       </c>
-      <c r="V15" s="34">
+      <c r="V15" s="30">
         <v>73</v>
       </c>
-      <c r="W15" s="43">
+      <c r="W15" s="49">
         <v>74</v>
       </c>
-      <c r="X15" s="43">
+      <c r="X15" s="49">
         <v>75</v>
       </c>
-      <c r="Y15" s="45">
+      <c r="Y15" s="50">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="2:26" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
@@ -1937,87 +1913,87 @@
       <c r="L16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O16" s="30" t="s">
+      <c r="O16" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="P16" s="31" t="s">
+      <c r="P16" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="R16" s="31" t="s">
+      <c r="Q16" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="S16" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="T16" s="30" t="s">
+      <c r="S16" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="T16" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="U16" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="V16" s="30" t="s">
+      <c r="U16" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="V16" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="W16" s="31" t="s">
+      <c r="W16" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="X16" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="36" t="s">
+      <c r="X16" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="32" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:27" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:27" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="24"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="23"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="7"/>
-      <c r="O17" s="33">
+      <c r="O17" s="29">
         <v>87</v>
       </c>
-      <c r="P17" s="34">
+      <c r="P17" s="30">
         <v>86</v>
       </c>
-      <c r="Q17" s="34">
+      <c r="Q17" s="30">
         <v>85</v>
       </c>
-      <c r="R17" s="34">
+      <c r="R17" s="30">
         <v>84</v>
       </c>
-      <c r="S17" s="34">
+      <c r="S17" s="30">
         <v>83</v>
       </c>
-      <c r="T17" s="33">
+      <c r="T17" s="29">
         <v>82</v>
       </c>
-      <c r="U17" s="35">
+      <c r="U17" s="31">
         <v>81</v>
       </c>
-      <c r="V17" s="33">
+      <c r="V17" s="29">
         <v>80</v>
       </c>
-      <c r="W17" s="34">
+      <c r="W17" s="30">
         <v>79</v>
       </c>
-      <c r="X17" s="35">
+      <c r="X17" s="31">
         <v>78</v>
       </c>
-      <c r="Y17" s="29">
+      <c r="Y17" s="28">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="2:27" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:27" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>1</v>
       </c>
@@ -2051,87 +2027,87 @@
       <c r="L18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O18" s="30" t="s">
+      <c r="O18" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="P18" s="31" t="s">
+      <c r="P18" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="Q18" s="31" t="s">
+      <c r="Q18" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="R18" s="31" t="s">
+      <c r="R18" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="S18" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="T18" s="30" t="s">
+      <c r="S18" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="T18" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="U18" s="31" t="s">
+      <c r="U18" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="V18" s="31" t="s">
+      <c r="V18" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="W18" s="31" t="s">
+      <c r="W18" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="X18" s="31" t="s">
+      <c r="X18" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="Y18" s="32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:27" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y18" s="55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="5"/>
       <c r="D19" s="15"/>
-      <c r="E19" s="28"/>
+      <c r="E19" s="27"/>
       <c r="F19" s="17"/>
       <c r="G19" s="15"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="22"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="21"/>
       <c r="J19" s="17"/>
       <c r="K19" s="5"/>
       <c r="L19" s="4"/>
-      <c r="O19" s="33">
+      <c r="O19" s="29">
         <v>88</v>
       </c>
-      <c r="P19" s="34">
+      <c r="P19" s="30">
         <v>89</v>
       </c>
-      <c r="Q19" s="34">
+      <c r="Q19" s="30">
         <v>90</v>
       </c>
-      <c r="R19" s="34">
+      <c r="R19" s="30">
         <v>91</v>
       </c>
-      <c r="S19" s="35">
+      <c r="S19" s="31">
         <v>92</v>
       </c>
-      <c r="T19" s="33">
+      <c r="T19" s="29">
         <v>93</v>
       </c>
-      <c r="U19" s="34">
+      <c r="U19" s="30">
         <v>94</v>
       </c>
-      <c r="V19" s="34">
+      <c r="V19" s="30">
         <v>95</v>
       </c>
-      <c r="W19" s="34">
+      <c r="W19" s="30">
         <v>96</v>
       </c>
-      <c r="X19" s="34">
+      <c r="X19" s="30">
         <v>97</v>
       </c>
-      <c r="Y19" s="35">
+      <c r="Y19" s="31">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="2:27" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:27" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -2163,91 +2139,91 @@
       <c r="L20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O20" s="30" t="s">
+      <c r="O20" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="P20" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="31" t="s">
+      <c r="P20" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="R20" s="31" t="s">
+      <c r="R20" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="S20" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="T20" s="30" t="s">
+      <c r="S20" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="T20" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="U20" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="V20" s="31" t="s">
+      <c r="U20" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="V20" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="W20" s="31" t="s">
+      <c r="W20" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="X20" s="31" t="s">
+      <c r="X20" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="Y20" s="32" t="s">
+      <c r="Y20" s="55" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:27" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="O21" s="33">
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="O21" s="29">
         <v>109</v>
       </c>
-      <c r="P21" s="34">
+      <c r="P21" s="30">
         <v>108</v>
       </c>
-      <c r="Q21" s="34">
+      <c r="Q21" s="30">
         <v>107</v>
       </c>
-      <c r="R21" s="34">
+      <c r="R21" s="30">
         <v>106</v>
       </c>
-      <c r="S21" s="35">
+      <c r="S21" s="31">
         <v>105</v>
       </c>
-      <c r="T21" s="33">
+      <c r="T21" s="29">
         <v>104</v>
       </c>
-      <c r="U21" s="34">
+      <c r="U21" s="30">
         <v>103</v>
       </c>
-      <c r="V21" s="34">
+      <c r="V21" s="30">
         <v>102</v>
       </c>
-      <c r="W21" s="34">
+      <c r="W21" s="30">
         <v>101</v>
       </c>
-      <c r="X21" s="34">
+      <c r="X21" s="30">
         <v>100</v>
       </c>
-      <c r="Y21" s="35">
+      <c r="Y21" s="31">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="2:27" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N22" s="20" t="s">
+    <row r="22" spans="2:27" ht="84.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Z22" s="20" t="s">
+      <c r="Z22" s="16" t="s">
         <v>36</v>
       </c>
       <c r="AA22">
@@ -2360,29 +2336,29 @@
       <c r="N4" s="19"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="38">
+      <c r="A5" s="34">
         <v>1.0416666666666701E-2</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37" t="s">
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37" t="s">
+      <c r="H5" s="33"/>
+      <c r="I5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37" t="s">
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33" t="s">
         <v>25</v>
       </c>
       <c r="N5" s="19"/>
@@ -2404,29 +2380,29 @@
       <c r="N6" s="19"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
+      <c r="A7" s="34">
         <v>1.38888888888889E-2</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37" t="s">
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37" t="s">
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37" t="s">
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33" t="s">
         <v>25</v>
       </c>
       <c r="N7" s="19"/>
@@ -2603,27 +2579,27 @@
       <c r="N15" s="19"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37" t="s">
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="37" t="s">
+      <c r="I16" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37" t="s">
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33" t="s">
         <v>29</v>
       </c>
       <c r="N16" s="19"/>

</xml_diff>